<commit_message>
study notes log4j web-front-end,js,jquery,
</commit_message>
<xml_diff>
--- a/study, research/spring cloud/demo spring cloud distributed system architecture.xlsx
+++ b/study, research/spring cloud/demo spring cloud distributed system architecture.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>eureka-server</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,6 +51,30 @@
   </si>
   <si>
     <t>路由器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>配置服务器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>config-server</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>配置客户端</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>config-client</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消息队列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rabbitMQ</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -75,7 +99,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -85,6 +109,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -103,7 +133,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -114,6 +144,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -410,9 +443,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.625" defaultRowHeight="24.95" customHeight="1"/>
   <cols>
@@ -483,6 +518,45 @@
       </c>
       <c r="C5" s="3">
         <v>8769</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="24.95" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3">
+        <v>8888</v>
+      </c>
+      <c r="D6" s="3">
+        <v>8889</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="24.95" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3">
+        <v>8899</v>
+      </c>
+      <c r="D7" s="3">
+        <v>8900</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="24.95" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="4">
+        <v>5672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>